<commit_message>
added json files for BV and QFT
</commit_message>
<xml_diff>
--- a/qc-app-oriented-benchmarks/json files converted to .xlsx files/DATA-quantum-fourier-transform-qiskit-qasm_simulator.xlsx
+++ b/qc-app-oriented-benchmarks/json files converted to .xlsx files/DATA-quantum-fourier-transform-qiskit-qasm_simulator.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Benchmark Results - Quantum Fourier Transform (1) - Qiskit" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Benchmark Results - Quantum Fourier Transform (3) - Qiskit" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Benchmark Results - Quantum Fourier Transform (2) - Qiskit" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Benchmark Results - Quantum Fourier Transform (3) - Qiskit" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2393,7 +2394,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2404,7 +2405,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Benchmark Results - Quantum Fourier Transform (3) - Qiskit</t>
+          <t>Benchmark Results - Quantum Fourier Transform (2) - Qiskit</t>
         </is>
       </c>
       <c r="B1" s="1" t="n"/>
@@ -2501,25 +2502,30 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
+          <t>max_memory_usage</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
           <t>std_create_times</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>std_elapsed_times</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>std_exec_times</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>std_fidelities</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>std_hf_fidelities</t>
         </is>
@@ -2535,10 +2541,2081 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>8</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.262</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="O4" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.058</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>9</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.452</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>16</v>
+      </c>
+      <c r="L5" t="n">
+        <v>6</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.327</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O5" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>13</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.538</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>27</v>
+      </c>
+      <c r="L6" t="n">
+        <v>12</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.357</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="O6" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C7" t="n">
+        <v>18</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.541</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>41</v>
+      </c>
+      <c r="L7" t="n">
+        <v>20</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.382</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O7" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C8" t="n">
+        <v>24</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.546</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>58</v>
+      </c>
+      <c r="L8" t="n">
+        <v>30</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.398</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.455</v>
+      </c>
+      <c r="O8" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>31</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.553</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>78</v>
+      </c>
+      <c r="L9" t="n">
+        <v>42</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O9" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C10" t="n">
+        <v>39</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.5590000000000001</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
+        <v>101</v>
+      </c>
+      <c r="L10" t="n">
+        <v>56</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.538</v>
+      </c>
+      <c r="O10" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C11" t="n">
+        <v>48</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.5669999999999999</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" t="n">
+        <v>127</v>
+      </c>
+      <c r="L11" t="n">
+        <v>72</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.428</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="O11" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C12" t="n">
+        <v>58</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" t="n">
+        <v>156</v>
+      </c>
+      <c r="L12" t="n">
+        <v>90</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.434</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O12" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="C13" t="n">
+        <v>69</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>188</v>
+      </c>
+      <c r="L13" t="n">
+        <v>110</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.439</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="O13" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="C14" t="n">
+        <v>81</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.615</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" t="n">
+        <v>223</v>
+      </c>
+      <c r="L14" t="n">
+        <v>132</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.647</v>
+      </c>
+      <c r="O14" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="C15" t="n">
+        <v>94</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="n">
+        <v>261</v>
+      </c>
+      <c r="L15" t="n">
+        <v>156</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="O15" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="C16" t="n">
+        <v>108</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.634</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>302</v>
+      </c>
+      <c r="L16" t="n">
+        <v>182</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.451</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.6840000000000001</v>
+      </c>
+      <c r="O16" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="C17" t="n">
+        <v>123</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.653</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" t="n">
+        <v>346</v>
+      </c>
+      <c r="L17" t="n">
+        <v>210</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.454</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O17" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="C18" t="n">
+        <v>139</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.707</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>393</v>
+      </c>
+      <c r="L18" t="n">
+        <v>240</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.457</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.714</v>
+      </c>
+      <c r="O18" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="C19" t="n">
+        <v>156</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>443</v>
+      </c>
+      <c r="L19" t="n">
+        <v>272</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.459</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="O19" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="C20" t="n">
+        <v>174</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.692</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.354</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" t="n">
+        <v>496</v>
+      </c>
+      <c r="L20" t="n">
+        <v>306</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.461</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.739</v>
+      </c>
+      <c r="O20" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.275</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="C21" t="n">
+        <v>193</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>552</v>
+      </c>
+      <c r="L21" t="n">
+        <v>342</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.463</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="O21" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="C22" t="n">
+        <v>213</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.181</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.074</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" t="n">
+        <v>611</v>
+      </c>
+      <c r="L22" t="n">
+        <v>380</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.465</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="O22" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.231</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="C23" t="n">
+        <v>234</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2.851</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.892</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" t="n">
+        <v>673</v>
+      </c>
+      <c r="L23" t="n">
+        <v>420</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.466</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.769</v>
+      </c>
+      <c r="O23" t="n">
+        <v>328.3125</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.152</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="C24" t="n">
+        <v>256</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2.807</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.569</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" t="n">
+        <v>738</v>
+      </c>
+      <c r="L24" t="n">
+        <v>462</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.468</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.778</v>
+      </c>
+      <c r="O24" t="n">
+        <v>364.6796875</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.168</v>
+      </c>
+      <c r="C25" t="n">
+        <v>279</v>
+      </c>
+      <c r="D25" t="n">
+        <v>4.736</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1.469</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" t="n">
+        <v>806</v>
+      </c>
+      <c r="L25" t="n">
+        <v>506</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.469</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.786</v>
+      </c>
+      <c r="O25" t="n">
+        <v>492.9765625</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.132</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="C26" t="n">
+        <v>303</v>
+      </c>
+      <c r="D26" t="n">
+        <v>6.609</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1.645</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" t="n">
+        <v>877</v>
+      </c>
+      <c r="L26" t="n">
+        <v>552</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.793</v>
+      </c>
+      <c r="O26" t="n">
+        <v>748.28125</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.674</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.604</v>
+      </c>
+      <c r="C27" t="n">
+        <v>328</v>
+      </c>
+      <c r="D27" t="n">
+        <v>12.342</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3.068</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" t="n">
+        <v>951</v>
+      </c>
+      <c r="L27" t="n">
+        <v>600</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.471</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1260.72265625</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.488</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>1.384</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1.073</v>
+      </c>
+      <c r="C28" t="n">
+        <v>354</v>
+      </c>
+      <c r="D28" t="n">
+        <v>24.853</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G28" t="n">
+        <v>6.087</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1</v>
+      </c>
+      <c r="J28" t="n">
+        <v>1</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1028</v>
+      </c>
+      <c r="L28" t="n">
+        <v>650</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.472</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.806</v>
+      </c>
+      <c r="O28" t="n">
+        <v>2285.125</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>2.945</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.191</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2.157</v>
+      </c>
+      <c r="C29" t="n">
+        <v>381</v>
+      </c>
+      <c r="D29" t="n">
+        <v>48.276</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G29" t="n">
+        <v>12.07</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" t="n">
+        <v>1</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1108</v>
+      </c>
+      <c r="L29" t="n">
+        <v>702</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.473</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.8120000000000001</v>
+      </c>
+      <c r="O29" t="n">
+        <v>4332.875</v>
+      </c>
+      <c r="P29" t="n">
+        <v>1.754</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>5.561</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0.074</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="C30" t="n">
+        <v>409</v>
+      </c>
+      <c r="D30" t="n">
+        <v>98.633</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G30" t="n">
+        <v>23.983</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1191</v>
+      </c>
+      <c r="L30" t="n">
+        <v>756</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.474</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.8179999999999999</v>
+      </c>
+      <c r="O30" t="n">
+        <v>8429.40234375</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>12.52</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0.128</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="C31" t="n">
+        <v>438</v>
+      </c>
+      <c r="D31" t="n">
+        <v>212.657</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G31" t="n">
+        <v>51.511</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1</v>
+      </c>
+      <c r="K31" t="n">
+        <v>1277</v>
+      </c>
+      <c r="L31" t="n">
+        <v>812</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.475</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.824</v>
+      </c>
+      <c r="O31" t="n">
+        <v>16620.81640625</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>27.26</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0.991</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="C32" t="n">
+        <v>468</v>
+      </c>
+      <c r="D32" t="n">
+        <v>437.289</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G32" t="n">
+        <v>108.795</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1366</v>
+      </c>
+      <c r="L32" t="n">
+        <v>870</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.476</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.829</v>
+      </c>
+      <c r="O32" t="n">
+        <v>33004.9140625</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>51.58</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0.749</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>36.633</v>
+      </c>
+      <c r="C33" t="n">
+        <v>499</v>
+      </c>
+      <c r="D33" t="n">
+        <v>356.262</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G33" t="n">
+        <v>214.622</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1458</v>
+      </c>
+      <c r="L33" t="n">
+        <v>930</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.477</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="O33" t="n">
+        <v>33004.9140625</v>
+      </c>
+      <c r="P33" t="n">
+        <v>29.903</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>60.282</v>
+      </c>
+      <c r="R33" t="n">
+        <v>2.634</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:U1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Benchmark Results - Quantum Fourier Transform (3) - Qiskit</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n"/>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="n"/>
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="n"/>
+      <c r="I1" s="1" t="n"/>
+      <c r="J1" s="1" t="n"/>
+      <c r="K1" s="1" t="n"/>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="n"/>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="n"/>
+      <c r="Q1" s="1" t="n"/>
+      <c r="R1" s="1" t="n"/>
+      <c r="S1" s="1" t="n"/>
+      <c r="T1" s="1" t="n"/>
+      <c r="U1" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>groups</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>avg_create_times</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>avg_depths</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>avg_elapsed_times</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>avg_exec_creating_times</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>avg_exec_running_times</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>avg_exec_times</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>avg_exec_validating_times</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>avg_fidelities</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>avg_hf_fidelities</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>avg_tr_depths</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>avg_tr_n2qs</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>avg_tr_xis</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>avg_xis</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>max_memory_usage</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>std_create_times</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>std_elapsed_times</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>std_exec_times</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>std_fidelities</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>std_hf_fidelities</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
         <v>5</v>
       </c>
       <c r="D4" t="n">
-        <v>0.036</v>
+        <v>0.098</v>
       </c>
       <c r="E4" t="n">
         <v>0.001</v>
@@ -2553,7 +4630,7 @@
         <v>0.001</v>
       </c>
       <c r="I4" t="n">
-        <v>0.999</v>
+        <v>0.498</v>
       </c>
       <c r="J4" t="n">
         <v>0.999</v>
@@ -2571,18 +4648,21 @@
         <v>0.2</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>209.77734375</v>
       </c>
       <c r="P4" t="n">
-        <v>0.007</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
       </c>
       <c r="S4" t="n">
+        <v>0.352</v>
+      </c>
+      <c r="T4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2593,13 +4673,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="C5" t="n">
         <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>0.328</v>
+        <v>0.309</v>
       </c>
       <c r="E5" t="n">
         <v>0.001</v>
@@ -2614,10 +4694,10 @@
         <v>0.001</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0.665</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="K5" t="n">
         <v>16</v>
@@ -2632,19 +4712,22 @@
         <v>0.333</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>210.33984375</v>
       </c>
       <c r="P5" t="n">
-        <v>0.137</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>0.116</v>
       </c>
       <c r="R5" t="n">
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>0.271</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.001</v>
       </c>
     </row>
     <row r="6">
@@ -2654,13 +4737,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="C6" t="n">
         <v>12</v>
       </c>
       <c r="D6" t="n">
-        <v>0.602</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="E6" t="n">
         <v>0.001</v>
@@ -2675,7 +4758,7 @@
         <v>0.001</v>
       </c>
       <c r="I6" t="n">
-        <v>0.999</v>
+        <v>0.998</v>
       </c>
       <c r="J6" t="n">
         <v>0.999</v>
@@ -2693,18 +4776,21 @@
         <v>0.429</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>210.71484375</v>
       </c>
       <c r="P6" t="n">
-        <v>0.019</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
       </c>
       <c r="S6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="T6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2715,13 +4801,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="C7" t="n">
         <v>17</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5669999999999999</v>
+        <v>0.572</v>
       </c>
       <c r="E7" t="n">
         <v>0.001</v>
@@ -2736,10 +4822,10 @@
         <v>0.001</v>
       </c>
       <c r="I7" t="n">
-        <v>0.995</v>
+        <v>0.663</v>
       </c>
       <c r="J7" t="n">
-        <v>0.995</v>
+        <v>0.996</v>
       </c>
       <c r="K7" t="n">
         <v>41</v>
@@ -2754,7 +4840,7 @@
         <v>0.5</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>211.08984375</v>
       </c>
       <c r="P7" t="n">
         <v>0.001</v>
@@ -2763,10 +4849,13 @@
         <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>0.002</v>
+        <v>0.271</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.001</v>
       </c>
     </row>
     <row r="8">
@@ -2782,7 +4871,7 @@
         <v>23</v>
       </c>
       <c r="D8" t="n">
-        <v>0.482</v>
+        <v>0.579</v>
       </c>
       <c r="E8" t="n">
         <v>0.001</v>
@@ -2797,7 +4886,7 @@
         <v>0.001</v>
       </c>
       <c r="I8" t="n">
-        <v>0.997</v>
+        <v>0.994</v>
       </c>
       <c r="J8" t="n">
         <v>0.997</v>
@@ -2815,19 +4904,1622 @@
         <v>0.556</v>
       </c>
       <c r="O8" t="n">
-        <v>0.001</v>
+        <v>211.27734375</v>
       </c>
       <c r="P8" t="n">
-        <v>0.094</v>
+        <v>0.001</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="T8" t="n">
         <v>0.002</v>
       </c>
-      <c r="S8" t="n">
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.587</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G9" t="n">
         <v>0.002</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.983</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.991</v>
+      </c>
+      <c r="K9" t="n">
+        <v>78</v>
+      </c>
+      <c r="L9" t="n">
+        <v>42</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.412</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O9" t="n">
+        <v>211.83984375</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C10" t="n">
+        <v>38</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.961</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.978</v>
+      </c>
+      <c r="K10" t="n">
+        <v>101</v>
+      </c>
+      <c r="L10" t="n">
+        <v>56</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.421</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.636</v>
+      </c>
+      <c r="O10" t="n">
+        <v>212.21484375</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="C11" t="n">
+        <v>47</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.621</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.951</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.972</v>
+      </c>
+      <c r="K11" t="n">
+        <v>127</v>
+      </c>
+      <c r="L11" t="n">
+        <v>72</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.429</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="O11" t="n">
+        <v>212.40234375</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="C12" t="n">
+        <v>57</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.639</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.967</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.974</v>
+      </c>
+      <c r="K12" t="n">
+        <v>156</v>
+      </c>
+      <c r="L12" t="n">
+        <v>90</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.435</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.6919999999999999</v>
+      </c>
+      <c r="O12" t="n">
+        <v>212.58984375</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="C13" t="n">
+        <v>68</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.654</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.957</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.964</v>
+      </c>
+      <c r="K13" t="n">
+        <v>188</v>
+      </c>
+      <c r="L13" t="n">
+        <v>110</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.714</v>
+      </c>
+      <c r="O13" t="n">
+        <v>213.15234375</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.017</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="C14" t="n">
+        <v>80</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.681</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.971</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.972</v>
+      </c>
+      <c r="K14" t="n">
+        <v>223</v>
+      </c>
+      <c r="L14" t="n">
+        <v>132</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.733</v>
+      </c>
+      <c r="O14" t="n">
+        <v>214.08984375</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="C15" t="n">
+        <v>93</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.964</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.966</v>
+      </c>
+      <c r="K15" t="n">
+        <v>261</v>
+      </c>
+      <c r="L15" t="n">
+        <v>156</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="O15" t="n">
+        <v>215.58984375</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="C16" t="n">
+        <v>107</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.318</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.954</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.956</v>
+      </c>
+      <c r="K16" t="n">
+        <v>302</v>
+      </c>
+      <c r="L16" t="n">
+        <v>182</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.452</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="O16" t="n">
+        <v>217.27734375</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.285</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="C17" t="n">
+        <v>122</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.872</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.843</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.964</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.965</v>
+      </c>
+      <c r="K17" t="n">
+        <v>346</v>
+      </c>
+      <c r="L17" t="n">
+        <v>210</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.455</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.778</v>
+      </c>
+      <c r="O17" t="n">
+        <v>223.08984375</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.283</v>
+      </c>
+      <c r="C18" t="n">
+        <v>138</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.939</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.665</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.965</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.965</v>
+      </c>
+      <c r="K18" t="n">
+        <v>393</v>
+      </c>
+      <c r="L18" t="n">
+        <v>240</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.457</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.789</v>
+      </c>
+      <c r="O18" t="n">
+        <v>232.77734375</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.227</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.162</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.204</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="C19" t="n">
+        <v>155</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.676</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.837</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.965</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.965</v>
+      </c>
+      <c r="K19" t="n">
+        <v>443</v>
+      </c>
+      <c r="L19" t="n">
+        <v>272</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.459</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O19" t="n">
+        <v>232.77734375</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.284</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.379</v>
+      </c>
+      <c r="C20" t="n">
+        <v>173</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.661</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.977</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.977</v>
+      </c>
+      <c r="K20" t="n">
+        <v>496</v>
+      </c>
+      <c r="L20" t="n">
+        <v>306</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.462</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="O20" t="n">
+        <v>235.29296875</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.304</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.337</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="C21" t="n">
+        <v>192</v>
+      </c>
+      <c r="D21" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.772</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.966</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.966</v>
+      </c>
+      <c r="K21" t="n">
+        <v>552</v>
+      </c>
+      <c r="L21" t="n">
+        <v>342</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.463</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.8179999999999999</v>
+      </c>
+      <c r="O21" t="n">
+        <v>246.99609375</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.315</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.158</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="C22" t="n">
+        <v>212</v>
+      </c>
+      <c r="D22" t="n">
+        <v>5.353</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.601</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" t="n">
+        <v>611</v>
+      </c>
+      <c r="L22" t="n">
+        <v>380</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.465</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.826</v>
+      </c>
+      <c r="O22" t="n">
+        <v>271.78125</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.103</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C23" t="n">
+        <v>233</v>
+      </c>
+      <c r="D23" t="n">
+        <v>5.94</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.729</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="K23" t="n">
+        <v>673</v>
+      </c>
+      <c r="L23" t="n">
+        <v>420</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.467</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="O23" t="n">
+        <v>303.37109375</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.161</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.587</v>
+      </c>
+      <c r="C24" t="n">
+        <v>255</v>
+      </c>
+      <c r="D24" t="n">
+        <v>7.155</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G24" t="n">
+        <v>2.031</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.973</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.973</v>
+      </c>
+      <c r="K24" t="n">
+        <v>738</v>
+      </c>
+      <c r="L24" t="n">
+        <v>462</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.468</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="O24" t="n">
+        <v>367.3125</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.473</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C25" t="n">
+        <v>278</v>
+      </c>
+      <c r="D25" t="n">
+        <v>9.734999999999999</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2.715</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="K25" t="n">
+        <v>806</v>
+      </c>
+      <c r="L25" t="n">
+        <v>506</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.469</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="O25" t="n">
+        <v>495.375</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.477</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="C26" t="n">
+        <v>302</v>
+      </c>
+      <c r="D26" t="n">
+        <v>13.231</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3.669</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="K26" t="n">
+        <v>877</v>
+      </c>
+      <c r="L26" t="n">
+        <v>552</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.471</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.852</v>
+      </c>
+      <c r="O26" t="n">
+        <v>751.40625</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.781</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0.002</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1.202</v>
+      </c>
+      <c r="C27" t="n">
+        <v>327</v>
+      </c>
+      <c r="D27" t="n">
+        <v>20.36</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5.337</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.996</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.996</v>
+      </c>
+      <c r="K27" t="n">
+        <v>951</v>
+      </c>
+      <c r="L27" t="n">
+        <v>600</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.472</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.857</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1263.5390625</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.973</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>1.767</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1.796</v>
+      </c>
+      <c r="C28" t="n">
+        <v>353</v>
+      </c>
+      <c r="D28" t="n">
+        <v>35.664</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G28" t="n">
+        <v>9.055999999999999</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.988</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.988</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1028</v>
+      </c>
+      <c r="L28" t="n">
+        <v>650</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.473</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.862</v>
+      </c>
+      <c r="O28" t="n">
+        <v>2287.89453125</v>
+      </c>
+      <c r="P28" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>3.634</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>3.033</v>
+      </c>
+      <c r="C29" t="n">
+        <v>380</v>
+      </c>
+      <c r="D29" t="n">
+        <v>67.82299999999999</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G29" t="n">
+        <v>16.691</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.997</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.997</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1108</v>
+      </c>
+      <c r="L29" t="n">
+        <v>702</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.474</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.867</v>
+      </c>
+      <c r="O29" t="n">
+        <v>4335.171875</v>
+      </c>
+      <c r="P29" t="n">
+        <v>2.441</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>7.897</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0.261</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0.002</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>5.513</v>
+      </c>
+      <c r="C30" t="n">
+        <v>408</v>
+      </c>
+      <c r="D30" t="n">
+        <v>136.723</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G30" t="n">
+        <v>32.979</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.993</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.993</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1191</v>
+      </c>
+      <c r="L30" t="n">
+        <v>756</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.475</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="O30" t="n">
+        <v>8431.32421875</v>
+      </c>
+      <c r="P30" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>16.797</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0.8090000000000001</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0.004</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>10.656</v>
+      </c>
+      <c r="C31" t="n">
+        <v>437</v>
+      </c>
+      <c r="D31" t="n">
+        <v>280.645</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G31" t="n">
+        <v>67.01000000000001</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.972</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.972</v>
+      </c>
+      <c r="K31" t="n">
+        <v>1277</v>
+      </c>
+      <c r="L31" t="n">
+        <v>812</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.475</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="O31" t="n">
+        <v>16624.0546875</v>
+      </c>
+      <c r="P31" t="n">
+        <v>8.688000000000001</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>35.804</v>
+      </c>
+      <c r="R31" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>21.001</v>
+      </c>
+      <c r="C32" t="n">
+        <v>467</v>
+      </c>
+      <c r="D32" t="n">
+        <v>611.7569999999999</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G32" t="n">
+        <v>138.93</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1366</v>
+      </c>
+      <c r="L32" t="n">
+        <v>870</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.476</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.879</v>
+      </c>
+      <c r="O32" t="n">
+        <v>33007.546875</v>
+      </c>
+      <c r="P32" t="n">
+        <v>17.135</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>87.124</v>
+      </c>
+      <c r="R32" t="n">
+        <v>8.558999999999999</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>42.462</v>
+      </c>
+      <c r="C33" t="n">
+        <v>498</v>
+      </c>
+      <c r="D33" t="n">
+        <v>493.692</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G33" t="n">
+        <v>308.996</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1458</v>
+      </c>
+      <c r="L33" t="n">
+        <v>930</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.477</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.882</v>
+      </c>
+      <c r="O33" t="n">
+        <v>33007.546875</v>
+      </c>
+      <c r="P33" t="n">
+        <v>34.631</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>94.699</v>
+      </c>
+      <c r="R33" t="n">
+        <v>26.907</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>